<commit_message>
About and indicators - cred, fossil fuel
</commit_message>
<xml_diff>
--- a/data/traffic_light_indicators_data.xlsx
+++ b/data/traffic_light_indicators_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maarten/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Almut B\Documents\GitHub\buildings-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A825303-F0B1-0141-A4DF-5165DB31DC9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7639A052-ECA7-481E-B1DB-5476C41DAC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27980" windowHeight="17540" xr2:uid="{C3AFBA72-B1BC-4A11-A93A-E672CAD481DA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C3AFBA72-B1BC-4A11-A93A-E672CAD481DA}"/>
   </bookViews>
   <sheets>
     <sheet name="limit_fossil_fuels_buildings" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="83">
   <si>
     <t>adopted</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>not submitted</t>
-  </si>
-  <si>
-    <t>submitted / not yet assessed</t>
   </si>
   <si>
     <t>submitted / assessed</t>
@@ -372,7 +369,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -388,7 +385,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -686,68 +683,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1AB4A6-8707-47B9-BBC4-4A31F53BD35D}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="18.33203125" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.6640625" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5" customWidth="1"/>
-    <col min="13" max="13" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" customWidth="1"/>
+    <col min="13" max="13" width="26.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -755,31 +752,31 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
         <v>51</v>
       </c>
-      <c r="J2" t="s">
-        <v>52</v>
-      </c>
       <c r="K2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -796,7 +793,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -813,7 +810,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -821,40 +818,40 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>59</v>
       </c>
-      <c r="G5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>60</v>
       </c>
-      <c r="M5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -868,16 +865,16 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -894,7 +891,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -911,7 +908,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -928,42 +925,42 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="5" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>28</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="L10" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -980,7 +977,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -994,22 +991,22 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1026,7 +1023,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1043,7 +1040,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1060,7 +1057,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1077,7 +1074,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1091,22 +1088,22 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L17" t="s">
-        <v>47</v>
-      </c>
       <c r="M17" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1123,7 +1120,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1140,7 +1137,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1148,40 +1145,40 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
         <v>48</v>
       </c>
-      <c r="D20" t="s">
-        <v>49</v>
-      </c>
       <c r="E20" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I20" t="s">
+        <v>47</v>
+      </c>
+      <c r="J20" t="s">
         <v>48</v>
       </c>
-      <c r="J20" t="s">
-        <v>49</v>
-      </c>
       <c r="K20" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1189,37 +1186,37 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1236,7 +1233,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1253,7 +1250,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1270,7 +1267,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1287,7 +1284,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1301,16 +1298,16 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1327,7 +1324,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>22</v>
       </c>
@@ -1335,37 +1332,37 @@
         <v>0</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>0</v>
       </c>
       <c r="F28" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="G28" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>82</v>
-      </c>
       <c r="J28" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>0</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1378,18 +1375,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06983421-EAFC-4095-94C9-21DB1E3C0C9C}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -1397,7 +1394,7 @@
         <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>31</v>
@@ -1409,10 +1406,10 @@
         <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1421,7 +1418,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1430,43 +1427,43 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1475,25 +1472,25 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1502,16 +1499,16 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1520,16 +1517,16 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1538,7 +1535,7 @@
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1547,52 +1544,52 @@
       </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1601,7 +1598,7 @@
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1610,7 +1607,7 @@
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1619,16 +1616,16 @@
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1637,25 +1634,25 @@
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>

</xml_diff>